<commit_message>
GBP YC bootstrapping - link RelinkableHandle to YC, and save expected rate values
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/GBP_YCONBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/GBP_YCONBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="9480" windowHeight="16440"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="9480" windowHeight="16440" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="3" r:id="rId1"/>
@@ -1385,7 +1385,7 @@
     <xf numFmtId="175" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="175" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1742,6 +1742,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="3"/>
@@ -2054,8 +2055,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2412,7 +2413,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="32">
-        <v>41614.558923611112</v>
+        <v>41614.586180555554</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="19"/>
@@ -2526,7 +2527,7 @@
       </c>
       <c r="D14" s="37" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_GBPYCON#0002</v>
+        <v>_GBPYCON#0000</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
@@ -4673,7 +4674,7 @@
       </c>
       <c r="L4" s="147" t="str">
         <f>_xll.qlEonia(K4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GBP_YCONRH__LiborON#0001</v>
+        <v>GBP_YCONRH__LiborON#0000</v>
       </c>
       <c r="M4" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -4734,7 +4735,7 @@
       </c>
       <c r="L6" s="133" t="str">
         <f>_xll.qlOISRateHelper(K6,B6,C6,J6,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_SWOIS#0001</v>
+        <v>GBP_YCONRH_SWOIS#0000</v>
       </c>
       <c r="M6" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -4788,7 +4789,7 @@
       </c>
       <c r="L7" s="133" t="str">
         <f>_xll.qlOISRateHelper(K7,B7,C7,J7,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_2WOIS#0001</v>
+        <v>GBP_YCONRH_2WOIS#0000</v>
       </c>
       <c r="M7" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -4842,7 +4843,7 @@
       </c>
       <c r="L8" s="133" t="str">
         <f>_xll.qlOISRateHelper(K8,B8,C8,J8,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_3WOIS#0001</v>
+        <v>GBP_YCONRH_3WOIS#0000</v>
       </c>
       <c r="M8" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -4896,7 +4897,7 @@
       </c>
       <c r="L9" s="133" t="str">
         <f>_xll.qlOISRateHelper(K9,B9,C9,J9,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_1MOIS#0001</v>
+        <v>GBP_YCONRH_1MOIS#0000</v>
       </c>
       <c r="M9" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -4950,7 +4951,7 @@
       </c>
       <c r="L10" s="133" t="str">
         <f>_xll.qlOISRateHelper(K10,B10,C10,J10,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_2MOIS#0001</v>
+        <v>GBP_YCONRH_2MOIS#0000</v>
       </c>
       <c r="M10" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -5004,7 +5005,7 @@
       </c>
       <c r="L11" s="133" t="str">
         <f>_xll.qlOISRateHelper(K11,B11,C11,J11,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_3MOIS#0001</v>
+        <v>GBP_YCONRH_3MOIS#0000</v>
       </c>
       <c r="M11" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -5058,7 +5059,7 @@
       </c>
       <c r="L12" s="133" t="str">
         <f>_xll.qlOISRateHelper(K12,B12,C12,J12,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_4MOIS#0001</v>
+        <v>GBP_YCONRH_4MOIS#0000</v>
       </c>
       <c r="M12" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -5112,7 +5113,7 @@
       </c>
       <c r="L13" s="133" t="str">
         <f>_xll.qlOISRateHelper(K13,B13,C13,J13,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_5MOIS#0001</v>
+        <v>GBP_YCONRH_5MOIS#0000</v>
       </c>
       <c r="M13" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -5166,7 +5167,7 @@
       </c>
       <c r="L14" s="133" t="str">
         <f>_xll.qlOISRateHelper(K14,B14,C14,J14,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_6MOIS#0001</v>
+        <v>GBP_YCONRH_6MOIS#0000</v>
       </c>
       <c r="M14" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -5220,7 +5221,7 @@
       </c>
       <c r="L15" s="133" t="str">
         <f>_xll.qlOISRateHelper(K15,B15,C15,J15,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_7MOIS#0001</v>
+        <v>GBP_YCONRH_7MOIS#0000</v>
       </c>
       <c r="M15" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -5274,7 +5275,7 @@
       </c>
       <c r="L16" s="133" t="str">
         <f>_xll.qlOISRateHelper(K16,B16,C16,J16,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_8MOIS#0001</v>
+        <v>GBP_YCONRH_8MOIS#0000</v>
       </c>
       <c r="M16" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -5328,7 +5329,7 @@
       </c>
       <c r="L17" s="133" t="str">
         <f>_xll.qlOISRateHelper(K17,B17,C17,J17,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_9MOIS#0001</v>
+        <v>GBP_YCONRH_9MOIS#0000</v>
       </c>
       <c r="M17" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -5382,7 +5383,7 @@
       </c>
       <c r="L18" s="133" t="str">
         <f>_xll.qlOISRateHelper(K18,B18,C18,J18,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_10MOIS#0001</v>
+        <v>GBP_YCONRH_10MOIS#0000</v>
       </c>
       <c r="M18" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -5436,7 +5437,7 @@
       </c>
       <c r="L19" s="133" t="str">
         <f>_xll.qlOISRateHelper(K19,B19,C19,J19,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_11MOIS#0001</v>
+        <v>GBP_YCONRH_11MOIS#0000</v>
       </c>
       <c r="M19" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -5490,7 +5491,7 @@
       </c>
       <c r="L20" s="133" t="str">
         <f>_xll.qlOISRateHelper(K20,B20,C20,J20,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_1YOIS#0001</v>
+        <v>GBP_YCONRH_1YOIS#0000</v>
       </c>
       <c r="M20" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -5544,7 +5545,7 @@
       </c>
       <c r="L21" s="133" t="str">
         <f>_xll.qlOISRateHelper(K21,B21,C21,J21,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_15MOIS#0001</v>
+        <v>GBP_YCONRH_15MOIS#0000</v>
       </c>
       <c r="M21" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -5598,7 +5599,7 @@
       </c>
       <c r="L22" s="133" t="str">
         <f>_xll.qlOISRateHelper(K22,B22,C22,J22,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_18MOIS#0001</v>
+        <v>GBP_YCONRH_18MOIS#0000</v>
       </c>
       <c r="M22" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -5652,7 +5653,7 @@
       </c>
       <c r="L23" s="133" t="str">
         <f>_xll.qlOISRateHelper(K23,B23,C23,J23,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_21MOIS#0001</v>
+        <v>GBP_YCONRH_21MOIS#0000</v>
       </c>
       <c r="M23" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -5706,7 +5707,7 @@
       </c>
       <c r="L24" s="133" t="str">
         <f>_xll.qlOISRateHelper(K24,B24,C24,J24,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_2YOIS#0001</v>
+        <v>GBP_YCONRH_2YOIS#0000</v>
       </c>
       <c r="M24" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -5760,7 +5761,7 @@
       </c>
       <c r="L25" s="133" t="str">
         <f>_xll.qlOISRateHelper(K25,B25,C25,J25,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_3YOIS#0001</v>
+        <v>GBP_YCONRH_3YOIS#0000</v>
       </c>
       <c r="M25" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -5814,7 +5815,7 @@
       </c>
       <c r="L26" s="133" t="str">
         <f>_xll.qlOISRateHelper(K26,B26,C26,J26,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_4YOIS#0001</v>
+        <v>GBP_YCONRH_4YOIS#0000</v>
       </c>
       <c r="M26" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -5868,7 +5869,7 @@
       </c>
       <c r="L27" s="133" t="str">
         <f>_xll.qlOISRateHelper(K27,B27,C27,J27,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_5YOIS#0001</v>
+        <v>GBP_YCONRH_5YOIS#0000</v>
       </c>
       <c r="M27" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -5922,7 +5923,7 @@
       </c>
       <c r="L28" s="133" t="str">
         <f>_xll.qlOISRateHelper(K28,B28,C28,J28,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_6YOIS#0001</v>
+        <v>GBP_YCONRH_6YOIS#0000</v>
       </c>
       <c r="M28" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -5976,7 +5977,7 @@
       </c>
       <c r="L29" s="133" t="str">
         <f>_xll.qlOISRateHelper(K29,B29,C29,J29,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_7YOIS#0001</v>
+        <v>GBP_YCONRH_7YOIS#0000</v>
       </c>
       <c r="M29" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -6030,7 +6031,7 @@
       </c>
       <c r="L30" s="133" t="str">
         <f>_xll.qlOISRateHelper(K30,B30,C30,J30,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_8YOIS#0001</v>
+        <v>GBP_YCONRH_8YOIS#0000</v>
       </c>
       <c r="M30" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -6084,7 +6085,7 @@
       </c>
       <c r="L31" s="133" t="str">
         <f>_xll.qlOISRateHelper(K31,B31,C31,J31,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_9YOIS#0001</v>
+        <v>GBP_YCONRH_9YOIS#0000</v>
       </c>
       <c r="M31" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -6138,7 +6139,7 @@
       </c>
       <c r="L32" s="133" t="str">
         <f>_xll.qlOISRateHelper(K32,B32,C32,J32,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_10YOIS#0001</v>
+        <v>GBP_YCONRH_10YOIS#0000</v>
       </c>
       <c r="M32" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -6192,7 +6193,7 @@
       </c>
       <c r="L33" s="133" t="str">
         <f>_xll.qlOISRateHelper(K33,B33,C33,J33,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_11YOIS#0001</v>
+        <v>GBP_YCONRH_11YOIS#0000</v>
       </c>
       <c r="M33" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -6246,7 +6247,7 @@
       </c>
       <c r="L34" s="133" t="str">
         <f>_xll.qlOISRateHelper(K34,B34,C34,J34,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_12YOIS#0001</v>
+        <v>GBP_YCONRH_12YOIS#0000</v>
       </c>
       <c r="M34" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -6300,7 +6301,7 @@
       </c>
       <c r="L35" s="133" t="str">
         <f>_xll.qlOISRateHelper(K35,B35,C35,J35,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_15YOIS#0001</v>
+        <v>GBP_YCONRH_15YOIS#0000</v>
       </c>
       <c r="M35" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -6354,7 +6355,7 @@
       </c>
       <c r="L36" s="133" t="str">
         <f>_xll.qlOISRateHelper(K36,B36,C36,J36,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_20YOIS#0001</v>
+        <v>GBP_YCONRH_20YOIS#0000</v>
       </c>
       <c r="M36" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -6408,7 +6409,7 @@
       </c>
       <c r="L37" s="133" t="str">
         <f>_xll.qlOISRateHelper(K37,B37,C37,J37,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_25YOIS#0001</v>
+        <v>GBP_YCONRH_25YOIS#0000</v>
       </c>
       <c r="M37" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -6462,7 +6463,7 @@
       </c>
       <c r="L38" s="133" t="str">
         <f>_xll.qlOISRateHelper(K38,B38,C38,J38,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_30YOIS#0001</v>
+        <v>GBP_YCONRH_30YOIS#0000</v>
       </c>
       <c r="M38" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -6534,7 +6535,7 @@
       </c>
       <c r="L40" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K40,B40,B41,J40,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCJAN11OIS#0001</v>
+        <v>GBP_YCONRH_MPCJAN11OIS#0000</v>
       </c>
       <c r="M40" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -6588,7 +6589,7 @@
       </c>
       <c r="L41" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K41,B41,B42,J41,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCFEB11OIS#0001</v>
+        <v>GBP_YCONRH_MPCFEB11OIS#0000</v>
       </c>
       <c r="M41" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -6642,7 +6643,7 @@
       </c>
       <c r="L42" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K42,B42,B43,J42,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCMAR11OIS#0001</v>
+        <v>GBP_YCONRH_MPCMAR11OIS#0000</v>
       </c>
       <c r="M42" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -6696,7 +6697,7 @@
       </c>
       <c r="L43" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K43,B43,B44,J43,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCAPR11OIS#0001</v>
+        <v>GBP_YCONRH_MPCAPR11OIS#0000</v>
       </c>
       <c r="M43" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L43)</f>
@@ -6750,7 +6751,7 @@
       </c>
       <c r="L44" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K44,B44,B45,J44,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCMAY11OIS#0001</v>
+        <v>GBP_YCONRH_MPCMAY11OIS#0000</v>
       </c>
       <c r="M44" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -6804,7 +6805,7 @@
       </c>
       <c r="L45" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K45,B45,B46,J45,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCJUN11OIS#0001</v>
+        <v>GBP_YCONRH_MPCJUN11OIS#0000</v>
       </c>
       <c r="M45" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -6858,7 +6859,7 @@
       </c>
       <c r="L46" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K46,B46,B47,J46,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCJUL11OIS#0001</v>
+        <v>GBP_YCONRH_MPCJUL11OIS#0000</v>
       </c>
       <c r="M46" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -6912,7 +6913,7 @@
       </c>
       <c r="L47" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K47,B47,B48,J47,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCAUG11OIS#0001</v>
+        <v>GBP_YCONRH_MPCAUG11OIS#0000</v>
       </c>
       <c r="M47" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -6966,7 +6967,7 @@
       </c>
       <c r="L48" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K48,B48,B49,J48,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCSEP11OIS#0001</v>
+        <v>GBP_YCONRH_MPCSEP11OIS#0000</v>
       </c>
       <c r="M48" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -7020,7 +7021,7 @@
       </c>
       <c r="L49" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K49,B49,B50,J49,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCOCT11OIS#0001</v>
+        <v>GBP_YCONRH_MPCOCT11OIS#0000</v>
       </c>
       <c r="M49" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -7074,7 +7075,7 @@
       </c>
       <c r="L50" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K50,B50,B51,J50,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCNOV11OIS#0001</v>
+        <v>GBP_YCONRH_MPCNOV11OIS#0000</v>
       </c>
       <c r="M50" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -7128,7 +7129,7 @@
       </c>
       <c r="L51" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K51,B51,B52,J51,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCDEC11OIS#0001</v>
+        <v>GBP_YCONRH_MPCDEC11OIS#0000</v>
       </c>
       <c r="M51" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L51)</f>
@@ -7182,7 +7183,7 @@
       </c>
       <c r="L52" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K52,B52,B53,J52,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCJAN12OIS#0001</v>
+        <v>GBP_YCONRH_MPCJAN12OIS#0000</v>
       </c>
       <c r="M52" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L52)</f>
@@ -7236,7 +7237,7 @@
       </c>
       <c r="L53" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K53,B53,B54,J53,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCFEB12OIS#0001</v>
+        <v>GBP_YCONRH_MPCFEB12OIS#0000</v>
       </c>
       <c r="M53" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L53)</f>
@@ -7290,7 +7291,7 @@
       </c>
       <c r="L54" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K54,B54,B55,J54,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCMAR12OIS#0001</v>
+        <v>GBP_YCONRH_MPCMAR12OIS#0000</v>
       </c>
       <c r="M54" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L54)</f>
@@ -7344,7 +7345,7 @@
       </c>
       <c r="L55" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K55,B55,B56,J55,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCAPR12OIS#0001</v>
+        <v>GBP_YCONRH_MPCAPR12OIS#0000</v>
       </c>
       <c r="M55" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L55)</f>
@@ -7398,7 +7399,7 @@
       </c>
       <c r="L56" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K56,B56,B57,J56,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCMAY12OIS#0001</v>
+        <v>GBP_YCONRH_MPCMAY12OIS#0000</v>
       </c>
       <c r="M56" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L56)</f>
@@ -7452,7 +7453,7 @@
       </c>
       <c r="L57" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K57,B57,B58,J57,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCJUN12OIS#0001</v>
+        <v>GBP_YCONRH_MPCJUN12OIS#0000</v>
       </c>
       <c r="M57" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L57)</f>
@@ -7506,7 +7507,7 @@
       </c>
       <c r="L58" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K58,B58,B59,J58,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCJUL12OIS#0001</v>
+        <v>GBP_YCONRH_MPCJUL12OIS#0000</v>
       </c>
       <c r="M58" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L58)</f>
@@ -7560,7 +7561,7 @@
       </c>
       <c r="L59" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K59,B59,B60,J59,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCAUG12OIS#0001</v>
+        <v>GBP_YCONRH_MPCAUG12OIS#0000</v>
       </c>
       <c r="M59" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L59)</f>
@@ -7614,7 +7615,7 @@
       </c>
       <c r="L60" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K60,B60,B61,J60,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCSEP12OIS#0001</v>
+        <v>GBP_YCONRH_MPCSEP12OIS#0000</v>
       </c>
       <c r="M60" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L60)</f>
@@ -7668,7 +7669,7 @@
       </c>
       <c r="L61" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K61,B61,B62,J61,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCOCT12OIS#0001</v>
+        <v>GBP_YCONRH_MPCOCT12OIS#0000</v>
       </c>
       <c r="M61" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L61)</f>
@@ -7722,7 +7723,7 @@
       </c>
       <c r="L62" s="133" t="str">
         <f>_xll.qlDatedOISRateHelper(K62,B62,B63,J62,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_MPCNOV12OIS#0001</v>
+        <v>GBP_YCONRH_MPCNOV12OIS#0000</v>
       </c>
       <c r="M62" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L62)</f>
@@ -13452,9 +13453,9 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet31"/>
-  <dimension ref="A1:J126"/>
+  <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -13474,7 +13475,7 @@
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="166" t="s">
         <v>36</v>
       </c>
@@ -13497,7 +13498,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>80</v>
       </c>
@@ -13530,8 +13531,11 @@
       <c r="I2" s="69" t="e">
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L2" s="168">
+        <v>4.1749999999999999E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>81</v>
       </c>
@@ -13567,8 +13571,11 @@
         <f>H3-H2</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L3" s="168">
+        <v>4.1749999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -13604,8 +13611,11 @@
         <f>H4-H3</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L4" s="168">
+        <v>4.1749999999999999E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
@@ -13641,8 +13651,11 @@
         <f>H5-H4</f>
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L5" s="168">
+        <v>4.1250000000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -13679,11 +13692,14 @@
         <f>H6-H5</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="168">
+        <v>4.0749999999999996E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>GBP_YCONRH_RateHelpersSelected#0001</v>
+        <v>GBP_YCONRH_RateHelpersSelected#0000</v>
       </c>
       <c r="B7" s="10" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -13718,8 +13734,11 @@
         <f>H7-H6</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L7" s="168">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C8" s="102" t="s">
         <v>128</v>
       </c>
@@ -13749,8 +13768,11 @@
         <f t="shared" ref="J8:J36" si="0">H8-H7</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L8" s="168">
+        <v>3.9500000000000004E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C9" s="102" t="s">
         <v>129</v>
       </c>
@@ -13780,8 +13802,11 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L9" s="168">
+        <v>3.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C10" s="102" t="s">
         <v>130</v>
       </c>
@@ -13811,8 +13836,11 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L10" s="168">
+        <v>3.8249999999999998E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" s="102" t="s">
         <v>131</v>
       </c>
@@ -13842,8 +13870,11 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L11" s="168">
+        <v>3.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C12" s="102" t="s">
         <v>132</v>
       </c>
@@ -13873,8 +13904,11 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L12" s="168">
+        <v>3.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C13" s="102" t="s">
         <v>133</v>
       </c>
@@ -13904,8 +13938,11 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L13" s="168">
+        <v>3.65E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C14" s="102" t="s">
         <v>134</v>
       </c>
@@ -13935,8 +13972,11 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L14" s="168">
+        <v>3.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C15" s="102" t="s">
         <v>135</v>
       </c>
@@ -13966,8 +14006,11 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L15" s="168">
+        <v>3.5750000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C16" s="102" t="s">
         <v>136</v>
       </c>
@@ -13997,8 +14040,11 @@
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L16" s="168">
+        <v>3.4749999999999998E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C17" s="102" t="s">
         <v>137</v>
       </c>
@@ -14028,8 +14074,11 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L17" s="168">
+        <v>3.4499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C18" s="102" t="s">
         <v>138</v>
       </c>
@@ -14059,8 +14108,11 @@
         <f t="shared" si="0"/>
         <v>182</v>
       </c>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L18" s="168">
+        <v>3.4749999999999998E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C19" s="102" t="s">
         <v>139</v>
       </c>
@@ -14090,8 +14142,11 @@
         <f t="shared" si="0"/>
         <v>365</v>
       </c>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L19" s="168">
+        <v>4.0499999999999998E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D20" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14119,7 +14174,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D21" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14147,7 +14202,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D22" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14175,7 +14230,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D23" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14203,7 +14258,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D24" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14231,7 +14286,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D25" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14259,7 +14314,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D26" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14287,7 +14342,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D27" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14315,7 +14370,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D28" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14343,7 +14398,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D29" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14371,7 +14426,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D30" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14399,7 +14454,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D31" s="62" t="e">
         <v>#N/A</v>
       </c>
@@ -14427,7 +14482,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D32" s="62" t="e">
         <v>#N/A</v>
       </c>

</xml_diff>